<commit_message>
đưa lên mạch điều khiển động cơ bước không có Driver
</commit_message>
<xml_diff>
--- a/Docs/SoDoGhepNoiModule.xlsx
+++ b/Docs/SoDoGhepNoiModule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>lcd16x2</t>
   </si>
@@ -123,6 +123,9 @@
   <si>
     <t>3 Phase không chổi
  than</t>
+  </si>
+  <si>
+    <t>StepMotor</t>
   </si>
 </sst>
 </file>
@@ -241,11 +244,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,7 +554,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -608,7 +611,7 @@
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="4"/>
@@ -624,7 +627,7 @@
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -674,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>

</xml_diff>

<commit_message>
thêm mạch StepMotor không có Driver
</commit_message>
<xml_diff>
--- a/Docs/SoDoGhepNoiModule.xlsx
+++ b/Docs/SoDoGhepNoiModule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="19440" windowHeight="7875"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="19440" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>